<commit_message>
Added sample data for Home Entity
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Sample data for entities.xlsx
+++ b/Design Data/Sample Data/Sample data for entities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02F393C-EF84-4BB2-B17F-57754B8983E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2345A281-8F4C-4CCE-A1E4-AD1822F4691B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
   <si>
     <t>UserName</t>
   </si>
@@ -239,6 +239,18 @@
   </si>
   <si>
     <t>Kenneth641@gmail.com</t>
+  </si>
+  <si>
+    <t>Water Intake in oz</t>
+  </si>
+  <si>
+    <t>Sleep Hours</t>
+  </si>
+  <si>
+    <t>Calorie Intake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Challenge Id </t>
   </si>
 </sst>
 </file>
@@ -578,7 +590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -1104,20 +1116,440 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8B5DDD-F88B-4D5E-A728-87E46A470DE7}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>10467</v>
+      </c>
+      <c r="C2">
+        <v>64</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>231</v>
+      </c>
+      <c r="F2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>16378</v>
+      </c>
+      <c r="C3">
+        <v>84</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>329</v>
+      </c>
+      <c r="F3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>16733</v>
+      </c>
+      <c r="C4">
+        <v>57</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>436</v>
+      </c>
+      <c r="F4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>13255</v>
+      </c>
+      <c r="C5">
+        <v>36</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>452</v>
+      </c>
+      <c r="F5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>16722</v>
+      </c>
+      <c r="C6">
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <v>6.5</v>
+      </c>
+      <c r="E6">
+        <v>322</v>
+      </c>
+      <c r="F6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>10278</v>
+      </c>
+      <c r="C7">
+        <v>98</v>
+      </c>
+      <c r="D7">
+        <v>5.5</v>
+      </c>
+      <c r="E7">
+        <v>544</v>
+      </c>
+      <c r="F7">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>11722</v>
+      </c>
+      <c r="C8">
+        <v>84</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>435</v>
+      </c>
+      <c r="F8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>16832</v>
+      </c>
+      <c r="C9">
+        <v>71</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>235</v>
+      </c>
+      <c r="F9">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>18928</v>
+      </c>
+      <c r="C10">
+        <v>65</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>289</v>
+      </c>
+      <c r="F10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>19028</v>
+      </c>
+      <c r="C11">
+        <v>58</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>267</v>
+      </c>
+      <c r="F11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>12563</v>
+      </c>
+      <c r="C12">
+        <v>91</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>489</v>
+      </c>
+      <c r="F12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>17383</v>
+      </c>
+      <c r="C13">
+        <v>101</v>
+      </c>
+      <c r="D13">
+        <v>8.5</v>
+      </c>
+      <c r="E13">
+        <v>654</v>
+      </c>
+      <c r="F13">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>16738</v>
+      </c>
+      <c r="C14">
+        <v>89</v>
+      </c>
+      <c r="D14">
+        <v>4.5</v>
+      </c>
+      <c r="E14">
+        <v>742</v>
+      </c>
+      <c r="F14">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>13893</v>
+      </c>
+      <c r="C15">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>341</v>
+      </c>
+      <c r="F15">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>10273</v>
+      </c>
+      <c r="C16">
+        <v>82</v>
+      </c>
+      <c r="D16">
+        <v>8.5</v>
+      </c>
+      <c r="E16">
+        <v>546</v>
+      </c>
+      <c r="F16">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>15839</v>
+      </c>
+      <c r="C17">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <v>7.5</v>
+      </c>
+      <c r="E17">
+        <v>178</v>
+      </c>
+      <c r="F17">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>14278</v>
+      </c>
+      <c r="C18">
+        <v>69</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>109</v>
+      </c>
+      <c r="F18">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>10297</v>
+      </c>
+      <c r="C19">
+        <v>75</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>681</v>
+      </c>
+      <c r="F19">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20">
+        <v>16382</v>
+      </c>
+      <c r="C20">
+        <v>81</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>201</v>
+      </c>
+      <c r="F20">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>9888</v>
+      </c>
+      <c r="C21">
+        <v>75</v>
+      </c>
+      <c r="D21">
+        <v>6.5</v>
+      </c>
+      <c r="E21">
+        <v>301</v>
+      </c>
+      <c r="F21">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sample data for Group Entity
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Sample data for entities.xlsx
+++ b/Design Data/Sample Data/Sample data for entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2345A281-8F4C-4CCE-A1E4-AD1822F4691B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBC8560-98C8-498D-844F-22CA1390F086}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="97">
   <si>
     <t>UserName</t>
   </si>
@@ -251,6 +251,78 @@
   </si>
   <si>
     <t xml:space="preserve">Challenge Id </t>
+  </si>
+  <si>
+    <t>Group Name</t>
+  </si>
+  <si>
+    <t>Creator</t>
+  </si>
+  <si>
+    <t>Created Date</t>
+  </si>
+  <si>
+    <t>Last edited</t>
+  </si>
+  <si>
+    <t>Avengers</t>
+  </si>
+  <si>
+    <t>Champions</t>
+  </si>
+  <si>
+    <t>Crew</t>
+  </si>
+  <si>
+    <t>Bosses</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t>Hustle</t>
+  </si>
+  <si>
+    <t>Icons</t>
+  </si>
+  <si>
+    <t>Legends</t>
+  </si>
+  <si>
+    <t>Masters</t>
+  </si>
+  <si>
+    <t>Ninjas</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Peak Performers</t>
+  </si>
+  <si>
+    <t>Rebels</t>
+  </si>
+  <si>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>Warriors</t>
+  </si>
+  <si>
+    <t>United</t>
+  </si>
+  <si>
+    <t>Squad</t>
+  </si>
+  <si>
+    <t>Rule Breakers</t>
+  </si>
+  <si>
+    <t>Monarchy</t>
+  </si>
+  <si>
+    <t>Best of the Best</t>
   </si>
 </sst>
 </file>
@@ -303,10 +375,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -591,7 +665,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -640,10 +714,10 @@
         <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>49</v>
@@ -663,10 +737,10 @@
         <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>50</v>
@@ -686,10 +760,10 @@
         <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>51</v>
@@ -709,10 +783,10 @@
         <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>52</v>
@@ -735,7 +809,7 @@
         <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>53</v>
@@ -755,7 +829,7 @@
         <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
         <v>48</v>
@@ -778,7 +852,7 @@
         <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
         <v>48</v>
@@ -801,10 +875,10 @@
         <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>56</v>
@@ -824,10 +898,10 @@
         <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>57</v>
@@ -847,10 +921,10 @@
         <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>58</v>
@@ -873,7 +947,7 @@
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>59</v>
@@ -893,7 +967,7 @@
         <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
         <v>48</v>
@@ -916,7 +990,7 @@
         <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>
@@ -939,7 +1013,7 @@
         <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
         <v>48</v>
@@ -962,10 +1036,10 @@
         <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>63</v>
@@ -985,10 +1059,10 @@
         <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>64</v>
@@ -1008,10 +1082,10 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>65</v>
@@ -1031,10 +1105,10 @@
         <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>66</v>
@@ -1054,10 +1128,10 @@
         <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>67</v>
@@ -1077,10 +1151,10 @@
         <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>68</v>
@@ -1118,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8B5DDD-F88B-4D5E-A728-87E46A470DE7}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -1560,13 +1634,317 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB4E68C-0CA9-4C18-8847-54715EEB10BD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.76113425925925926</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.63359953703703698</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.67899305555555556</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.59625000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.50706018518518514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.42372685185185183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.46609953703703705</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.50847222222222221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.55084490740740744</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.59321759259259255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.63559027777777777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.67868055555555562</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.72105324074074073</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.76342592592592595</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.80579861111111117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.84817129629629628</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.89054398148148151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.93291666666666673</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.9758796296296296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.6793865740740741</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added sample data for Group Member Entity
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Sample data for entities.xlsx
+++ b/Design Data/Sample Data/Sample data for entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBC8560-98C8-498D-844F-22CA1390F086}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76784710-29BF-4F54-9F9D-C880DCB97504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="105">
   <si>
     <t>UserName</t>
   </si>
@@ -323,6 +323,30 @@
   </si>
   <si>
     <t>Best of the Best</t>
+  </si>
+  <si>
+    <t>Date Invited</t>
+  </si>
+  <si>
+    <t>Date Accepted Invite</t>
+  </si>
+  <si>
+    <t>Date Rejected Invite</t>
+  </si>
+  <si>
+    <t>Date Left Group</t>
+  </si>
+  <si>
+    <t>Verification Code</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>9/102020</t>
   </si>
 </sst>
 </file>
@@ -1636,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB4E68C-0CA9-4C18-8847-54715EEB10BD}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1684,7 +1708,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D3" s="4">
         <v>0.63359953703703698</v>
@@ -1698,7 +1722,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="3">
-        <v>44084</v>
+        <v>44086</v>
       </c>
       <c r="D4" s="4">
         <v>0.67899305555555556</v>
@@ -1712,7 +1736,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3">
-        <v>44084</v>
+        <v>44083</v>
       </c>
       <c r="D5" s="4">
         <v>0.59625000000000006</v>
@@ -1726,7 +1750,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="3">
-        <v>44084</v>
+        <v>44086</v>
       </c>
       <c r="D6" s="4">
         <v>0.50706018518518514</v>
@@ -1740,7 +1764,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="3">
-        <v>44084</v>
+        <v>44088</v>
       </c>
       <c r="D7" s="4">
         <v>0.42372685185185183</v>
@@ -1754,7 +1778,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="3">
-        <v>44084</v>
+        <v>44082</v>
       </c>
       <c r="D8" s="4">
         <v>0.46609953703703705</v>
@@ -1768,7 +1792,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3">
-        <v>44084</v>
+        <v>44083</v>
       </c>
       <c r="D9" s="4">
         <v>0.50847222222222221</v>
@@ -1796,7 +1820,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="3">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D11" s="4">
         <v>0.59321759259259255</v>
@@ -1810,7 +1834,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="3">
-        <v>44084</v>
+        <v>44086</v>
       </c>
       <c r="D12" s="4">
         <v>0.63559027777777777</v>
@@ -1824,7 +1848,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="3">
-        <v>44084</v>
+        <v>44087</v>
       </c>
       <c r="D13" s="4">
         <v>0.67868055555555562</v>
@@ -1838,7 +1862,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="3">
-        <v>44084</v>
+        <v>44089</v>
       </c>
       <c r="D14" s="4">
         <v>0.72105324074074073</v>
@@ -1852,7 +1876,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="3">
-        <v>44084</v>
+        <v>44083</v>
       </c>
       <c r="D15" s="4">
         <v>0.76342592592592595</v>
@@ -1866,7 +1890,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="3">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D16" s="4">
         <v>0.80579861111111117</v>
@@ -1894,7 +1918,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="3">
-        <v>44084</v>
+        <v>44086</v>
       </c>
       <c r="D18" s="4">
         <v>0.89054398148148151</v>
@@ -1908,7 +1932,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="3">
-        <v>44084</v>
+        <v>44086</v>
       </c>
       <c r="D19" s="4">
         <v>0.93291666666666673</v>
@@ -1936,7 +1960,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="3">
-        <v>44084</v>
+        <v>44082</v>
       </c>
       <c r="D21" s="4">
         <v>0.6793865740740741</v>
@@ -1950,24 +1974,241 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493B3549-B49E-4EC2-836B-66FF9983BD48}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>44084</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>44085</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44086</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44087</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>44086</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>44083</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>44086</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44088</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>44088</v>
+      </c>
+      <c r="B7" s="3">
+        <v>44090</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>44082</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44084</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>44083</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>44084</v>
+      </c>
+      <c r="B10" s="3">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>44085</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44087</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>44086</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44089</v>
+      </c>
+      <c r="D12" s="3">
+        <v>44094</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>44087</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44091</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>44089</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44089</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>44083</v>
+      </c>
+      <c r="B15" s="3">
+        <v>44083</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>44085</v>
+      </c>
+      <c r="B16" s="3">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>44084</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>44086</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44087</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>44086</v>
+      </c>
+      <c r="C19" s="3">
+        <v>44087</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>44084</v>
+      </c>
+      <c r="B20" s="3">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>44082</v>
+      </c>
+      <c r="B21" s="3">
+        <v>44083</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3FC752-2CCC-4ADA-BD93-3CC74B8D634B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added sample data for Reset Password Entity
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Sample data for entities.xlsx
+++ b/Design Data/Sample Data/Sample data for entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76784710-29BF-4F54-9F9D-C880DCB97504}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FB43BC-3738-42C4-9218-0784F26B05A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
   <si>
     <t>UserName</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t>9/102020</t>
+  </si>
+  <si>
+    <t>Johnny234</t>
+  </si>
+  <si>
+    <t>Christopher341</t>
+  </si>
+  <si>
+    <t>Kenneth231</t>
   </si>
 </sst>
 </file>
@@ -689,7 +698,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1976,7 +1985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{493B3549-B49E-4EC2-836B-66FF9983BD48}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -2182,14 +2191,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3FC752-2CCC-4ADA-BD93-3CC74B8D634B}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="24.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2208,7 +2218,259 @@
         <v>103</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>127</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>131</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>133</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>141</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>143</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14">
+        <v>145</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>147</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16">
+        <v>149</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <v>153</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19">
+        <v>155</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20">
+        <v>157</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21">
+        <v>159</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3E500F6C-B005-4FD5-8341-0D4C4A577D27}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{BFB5CEBE-6EB3-4570-8965-2DCB8FB32D38}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{9EAAF5F8-91C6-4EF4-9859-4BF770C9F797}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{646DD1EC-D6F8-4A8F-87C9-A2B06877C90B}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{55B87998-C303-4D7D-BEAF-25AE81CF0C4B}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{CB1055F4-3CEB-4A08-B4E6-1E69BAA61ACA}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{D47F77C1-1A5C-45A4-B98C-D619872E4FBF}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{6B0A71EC-7E8F-4C35-94CE-98F93A7328FA}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{965153E3-7822-4672-9FA9-5ECB188BCE68}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{671C8B7F-CE8C-44B6-8639-C8DA1E203EF5}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{DCF8ED35-D9DD-4723-B47B-76E692EE915C}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{895E4CA8-8A92-4A57-86DF-EEBFADF626D0}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{69A3ABD1-BD14-45DA-A50D-D10F01D0F840}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{B2A18679-5418-45E7-BDDC-39DA803A3AE1}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{68833912-76FC-489C-81B9-A4CA3F3FBD65}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{BE93573C-0BF2-437C-9D44-3397269A53B8}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{E2ECD02D-96EC-439D-8E28-7832B9CBED1B}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{4F6E11E7-5BE1-47CB-BD9F-4B36DEA13662}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{F93FA330-E38A-4B94-8646-F15A6B2D8B55}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{84BFF350-6702-4C0F-84D4-9F8DBD1DE976}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added data for Profile Entity
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Sample data for entities.xlsx
+++ b/Design Data/Sample Data/Sample data for entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FB43BC-3738-42C4-9218-0784F26B05A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602984EB-C0D9-4B86-91A0-7B1D14E7628B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="145">
   <si>
     <t>UserName</t>
   </si>
@@ -356,6 +356,117 @@
   </si>
   <si>
     <t>Kenneth231</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>ActivityId</t>
+  </si>
+  <si>
+    <t>Medical Condition</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Weigth(lbs)</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Better</t>
+  </si>
+  <si>
+    <t>Worst</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Adequate</t>
+  </si>
+  <si>
+    <t>fine</t>
+  </si>
+  <si>
+    <t>in order</t>
+  </si>
+  <si>
+    <t>Fine</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Argentia</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Ireland</t>
   </si>
 </sst>
 </file>
@@ -698,7 +809,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2193,7 +2304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3FC752-2CCC-4ADA-BD93-3CC74B8D634B}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -2477,13 +2588,570 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BCB583-04A0-41CC-9CF1-170A1216D898}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2">
+        <v>8938398373</v>
+      </c>
+      <c r="D2">
+        <v>175</v>
+      </c>
+      <c r="E2">
+        <v>5.5</v>
+      </c>
+      <c r="F2">
+        <v>1091</v>
+      </c>
+      <c r="G2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3">
+        <v>5685893789</v>
+      </c>
+      <c r="D3">
+        <v>167</v>
+      </c>
+      <c r="E3">
+        <v>5.6</v>
+      </c>
+      <c r="F3">
+        <v>1091</v>
+      </c>
+      <c r="G3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4">
+        <v>5373638789</v>
+      </c>
+      <c r="D4">
+        <v>167</v>
+      </c>
+      <c r="E4">
+        <v>5.7</v>
+      </c>
+      <c r="F4">
+        <v>1092</v>
+      </c>
+      <c r="G4" t="s">
+        <v>120</v>
+      </c>
+      <c r="H4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5">
+        <v>2453683936</v>
+      </c>
+      <c r="D5">
+        <v>189</v>
+      </c>
+      <c r="E5">
+        <v>5.8</v>
+      </c>
+      <c r="F5">
+        <v>1093</v>
+      </c>
+      <c r="G5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6">
+        <v>5478363889</v>
+      </c>
+      <c r="D6">
+        <v>110</v>
+      </c>
+      <c r="E6">
+        <v>5.9</v>
+      </c>
+      <c r="F6">
+        <v>1094</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7">
+        <v>5378227889</v>
+      </c>
+      <c r="D7">
+        <v>111</v>
+      </c>
+      <c r="E7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F7">
+        <v>1095</v>
+      </c>
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8">
+        <v>4362781811</v>
+      </c>
+      <c r="D8">
+        <v>134</v>
+      </c>
+      <c r="E8">
+        <v>5.4</v>
+      </c>
+      <c r="F8">
+        <v>1096</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9">
+        <v>3252672819</v>
+      </c>
+      <c r="D9">
+        <v>142</v>
+      </c>
+      <c r="E9">
+        <v>5.5</v>
+      </c>
+      <c r="F9">
+        <v>1097</v>
+      </c>
+      <c r="G9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10">
+        <v>4362782829</v>
+      </c>
+      <c r="D10">
+        <v>152</v>
+      </c>
+      <c r="E10">
+        <v>5.2</v>
+      </c>
+      <c r="F10">
+        <v>1098</v>
+      </c>
+      <c r="G10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11">
+        <v>1324627856</v>
+      </c>
+      <c r="D11">
+        <v>162</v>
+      </c>
+      <c r="E11">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F11">
+        <v>1099</v>
+      </c>
+      <c r="G11" t="s">
+        <v>120</v>
+      </c>
+      <c r="H11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12">
+        <v>1452672829</v>
+      </c>
+      <c r="D12">
+        <v>178</v>
+      </c>
+      <c r="E12">
+        <v>5.5</v>
+      </c>
+      <c r="F12">
+        <v>1100</v>
+      </c>
+      <c r="G12" t="s">
+        <v>125</v>
+      </c>
+      <c r="H12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13">
+        <v>2453782829</v>
+      </c>
+      <c r="D13">
+        <v>181</v>
+      </c>
+      <c r="E13">
+        <v>5.8</v>
+      </c>
+      <c r="F13">
+        <v>1081</v>
+      </c>
+      <c r="G13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14">
+        <v>5464748843</v>
+      </c>
+      <c r="D14">
+        <v>192</v>
+      </c>
+      <c r="E14">
+        <v>5.2</v>
+      </c>
+      <c r="F14">
+        <v>1082</v>
+      </c>
+      <c r="G14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15">
+        <v>2627838934</v>
+      </c>
+      <c r="D15">
+        <v>136</v>
+      </c>
+      <c r="E15">
+        <v>5.9</v>
+      </c>
+      <c r="F15">
+        <v>1083</v>
+      </c>
+      <c r="G15" t="s">
+        <v>121</v>
+      </c>
+      <c r="H15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16">
+        <v>4263783993</v>
+      </c>
+      <c r="D16">
+        <v>178</v>
+      </c>
+      <c r="E16">
+        <v>5.3</v>
+      </c>
+      <c r="F16">
+        <v>1084</v>
+      </c>
+      <c r="G16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17">
+        <v>4262781999</v>
+      </c>
+      <c r="D17">
+        <v>156</v>
+      </c>
+      <c r="E17">
+        <v>5.8</v>
+      </c>
+      <c r="F17">
+        <v>1085</v>
+      </c>
+      <c r="G17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18">
+        <v>1226367788</v>
+      </c>
+      <c r="D18">
+        <v>128</v>
+      </c>
+      <c r="E18">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F18">
+        <v>1086</v>
+      </c>
+      <c r="G18" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19">
+        <v>4352678281</v>
+      </c>
+      <c r="D19">
+        <v>119</v>
+      </c>
+      <c r="E19">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="F19">
+        <v>1087</v>
+      </c>
+      <c r="G19" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20">
+        <v>3563378381</v>
+      </c>
+      <c r="D20">
+        <v>110</v>
+      </c>
+      <c r="E20">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F20">
+        <v>1089</v>
+      </c>
+      <c r="G20" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21">
+        <v>2452672782</v>
+      </c>
+      <c r="D21">
+        <v>111</v>
+      </c>
+      <c r="E21">
+        <v>5.7</v>
+      </c>
+      <c r="F21">
+        <v>1090</v>
+      </c>
+      <c r="G21" t="s">
+        <v>123</v>
+      </c>
+      <c r="H21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
created sample data for Activity entity
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Sample data for entities.xlsx
+++ b/Design Data/Sample Data/Sample data for entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602984EB-C0D9-4B86-91A0-7B1D14E7628B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6BC974-5A2B-4C6E-A881-D93A17D3579B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="157">
   <si>
     <t>UserName</t>
   </si>
@@ -467,6 +467,42 @@
   </si>
   <si>
     <t>Ireland</t>
+  </si>
+  <si>
+    <t>Activity Name</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Last Edited</t>
+  </si>
+  <si>
+    <t>Climbing</t>
+  </si>
+  <si>
+    <t>Swimming</t>
+  </si>
+  <si>
+    <t>Hiking</t>
+  </si>
+  <si>
+    <t>Rock Climbing</t>
+  </si>
+  <si>
+    <t>Walking</t>
+  </si>
+  <si>
+    <t>Dancing</t>
+  </si>
+  <si>
+    <t>Jogging</t>
+  </si>
+  <si>
+    <t>Running</t>
+  </si>
+  <si>
+    <t>Bicycle Riding</t>
   </si>
 </sst>
 </file>
@@ -809,7 +845,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1781,7 +1817,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2590,8 +2626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BCB583-04A0-41CC-9CF1-170A1216D898}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3157,13 +3193,383 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416BFC41-9C5D-43DC-823F-34B7584A6B33}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1091</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44094</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.50706018518518514</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1091</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44095</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.42372685185185183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>1092</v>
+      </c>
+      <c r="B4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3">
+        <v>44096</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.46609953703703705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>1093</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44094</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.50847222222222221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1094</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44095</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.55084490740740744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>1095</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44096</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.59321759259259255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1096</v>
+      </c>
+      <c r="B8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3">
+        <v>44097</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.63559027777777777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1097</v>
+      </c>
+      <c r="B9" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3">
+        <v>44094</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.67868055555555562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1098</v>
+      </c>
+      <c r="B10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="3">
+        <v>44096</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.72105324074074073</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1099</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="3">
+        <v>44096</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.76342592592592595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1100</v>
+      </c>
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3">
+        <v>44094</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.80579861111111117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1081</v>
+      </c>
+      <c r="B13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="3">
+        <v>44095</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.84817129629629628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1082</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3">
+        <v>44097</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.89054398148148151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1083</v>
+      </c>
+      <c r="B15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3">
+        <v>44098</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.93291666666666673</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1084</v>
+      </c>
+      <c r="B16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>44094</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.9758796296296296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1085</v>
+      </c>
+      <c r="B17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="3">
+        <v>44094</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.6793865740740741</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1086</v>
+      </c>
+      <c r="B18" t="s">
+        <v>155</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="3">
+        <v>44094</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.46609953703703705</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1087</v>
+      </c>
+      <c r="B19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3">
+        <v>44095</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.50847222222222221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1089</v>
+      </c>
+      <c r="B20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="3">
+        <v>44095</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.55084490740740744</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1090</v>
+      </c>
+      <c r="B21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3">
+        <v>44096</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.59321759259259255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E22" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added sample data for Challenge Entity
</commit_message>
<xml_diff>
--- a/Design Data/Sample Data/Sample data for entities.xlsx
+++ b/Design Data/Sample Data/Sample data for entities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S538106\Desktop\gdp_health_app\Design Data\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6BC974-5A2B-4C6E-A881-D93A17D3579B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4063EA-BEA4-49F4-A2F0-63AAED475EED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USER" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="165">
   <si>
     <t>UserName</t>
   </si>
@@ -503,6 +503,30 @@
   </si>
   <si>
     <t>Bicycle Riding</t>
+  </si>
+  <si>
+    <t>Challenge Name</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Calorie</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Diet</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Hydration</t>
+  </si>
+  <si>
+    <t>13:11:10 PM</t>
   </si>
 </sst>
 </file>
@@ -3195,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416BFC41-9C5D-43DC-823F-34B7584A6B33}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3575,12 +3599,316 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9F54AA-FF8F-4D91-92A7-2BA1F073E2C9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44095</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3">
+        <v>44094</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.49733796296296301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44095</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.42443287037037036</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44095</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.50847222222222221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44096</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.55084490740740744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="3">
+        <v>44096</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.63488425925925929</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44097</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.63559027777777777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44096</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.67868055555555562</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44094</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.72105324074074073</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44096</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.76342592592592595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3">
+        <v>44095</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.80579861111111117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3">
+        <v>44096</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.84817129629629628</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3">
+        <v>44097</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.89054398148148151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3">
+        <v>44098</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.93291666666666673</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3">
+        <v>44095</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.9758796296296296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44094</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.6793865740740741</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3">
+        <v>44096</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.46609953703703705</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="3">
+        <v>44094</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.50847222222222221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="3">
+        <v>44095</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.55084490740740744</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="3">
+        <v>44097</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.59321759259259255</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>